<commit_message>
added Hopfenberg and avoid negative numbers
</commit_message>
<xml_diff>
--- a/examples_sheets/Hopfenberg.xlsx
+++ b/examples_sheets/Hopfenberg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Projects\diffusionpy\examples_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23802682-A904-4E26-8C95-5C92C8B3A66A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F20A6C-040A-4722-9089-BC815F011B6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{4213FBD1-A38E-488F-88A4-D493D73D5A89}"/>
   </bookViews>
@@ -22,6 +22,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>t/s</t>
+  </si>
+  <si>
+    <t>L/m</t>
+  </si>
+  <si>
+    <t>D/m^2/s</t>
+  </si>
+  <si>
+    <t>ws0</t>
+  </si>
+  <si>
+    <t>ws8</t>
+  </si>
+  <si>
+    <t>kr</t>
+  </si>
+  <si>
+    <t>mf</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>wcrank/-</t>
+  </si>
+  <si>
+    <t>wHopfenberg/-</t>
+  </si>
+  <si>
+    <t>kf=D/L^2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -89,73 +127,43 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1664260717410319E-2"/>
+          <c:y val="7.407407407407407E-2"/>
+          <c:w val="0.8648912948381452"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$8:$I$15</c:f>
+              <c:f>Tabelle1!$A$4:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -179,47 +187,603 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$K$8:$K$15</c:f>
+              <c:f>Tabelle1!$B$4:$B$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.10052077451625771</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.25032076310799489</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.28250938855406649</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.29366561242814843</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.29768296281241674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.29914938943151953</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.29968731803865895</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.29988500320540673</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.29995769943619105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29998443908663064</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.29999427554032548</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.29999789409986005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.29999922528410666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29999971499814942</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29999989515370551</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.29999996142920743</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.29999998581059889</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.2999999947800111</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.29999999807967342</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.29999999929355137</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.29999999974011204</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.29999999990439258</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.29999999996482801</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.29999999998706095</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.29999999999524002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.29999999999824895</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.29999999999935584</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.29999999999976307</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.29999999999991284</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29999999999996796</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.29999999999998822</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.29999999999999571</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.29999999999999843</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.29999999999999938</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.29999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3AD6-4B49-BC71-8C8F7CD4CDE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$4:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$4:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>0.10026046261495791</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18715630764909605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21106650111708256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22212005547010225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2285484250723385</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23317901886556028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2370269677519623</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24046720943024608</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24364372940945142</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24661621405008735</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.24941316087209395</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25205121852277912</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25454226774569666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25689603935205052</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25912110317634063</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26122525995674178</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26321571245463549</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26509915333004203</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2668818202277834</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.26856953674827427</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.27016774635104346</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.27168154196806199</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.27311569252019052</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.27447466693042666</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.27576265599015631</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27698359233181136</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27814116870978345</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27923885476039506</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28027991238967825</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28126740992027205</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.28220423511412168</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.28309310717505093</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.28393658782425996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.28473709153210258</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.2854968949809441</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.28621814582631872</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.28690287081689186</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.28755298332776219</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.28817029035632741</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.28875649902520778</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.28931322263249476</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.28984198628582208</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.29034423215337501</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.29082132436193064</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.29127455356930265</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.29170514123612584</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.29211424361971899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A60D-4934-889B-96081AAFA5B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -300,6 +864,7 @@
         <c:axId val="2131825231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -970,16 +1535,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>678006</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15153</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>678006</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>91353</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1304,247 +1869,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA87F59-7AD7-45BC-ABE8-9DF063DDE70E}">
-  <dimension ref="I5:P20"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E35" sqref="E7:S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="K5" s="1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L5" s="1">
+      <c r="H2" s="1">
         <v>9.9999999999999994E-12</v>
       </c>
-      <c r="M5">
+      <c r="I2">
         <v>0.1</v>
       </c>
-      <c r="N5">
+      <c r="J2">
         <v>0.3</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="K6" s="1">
-        <f>L5/K5^2</f>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f t="array" ref="B4:B50">_xll.crank_xl(A4:A50,G2,H2,I2,J2)</f>
+        <v>0.10052077451625771</v>
+      </c>
+      <c r="C4">
+        <f t="array" ref="C4:C50">_xll.BHX_xloil(A4:A50,G4,H4,I2,J2,K2,L2)</f>
+        <v>0.10026046261495791</v>
+      </c>
+      <c r="G4" s="1">
+        <f>H2/G2^2</f>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="L6">
-        <v>0.1</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="e">
-        <f t="array" aca="1" ref="K8:O15" ca="1">_xll.crank_xl(I8:I15,K5,L5,M5,N5)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L8" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M8" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N8" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O8" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I9">
+      <c r="H4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>10</v>
       </c>
-      <c r="K9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="10" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I10">
+      <c r="B5">
+        <v>0.25032076310799489</v>
+      </c>
+      <c r="C5">
+        <v>0.18715630764909605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>20</v>
       </c>
-      <c r="K10" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L10" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M10" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N10" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O10" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="11" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I11">
+      <c r="B6">
+        <v>0.28250938855406649</v>
+      </c>
+      <c r="C6">
+        <v>0.21106650111708256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>30</v>
       </c>
-      <c r="K11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="12" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I12">
+      <c r="B7">
+        <v>0.29366561242814843</v>
+      </c>
+      <c r="C7">
+        <v>0.22212005547010225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>40</v>
       </c>
-      <c r="K12" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L12" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M12" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N12" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O12" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="13" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I13">
+      <c r="B8">
+        <v>0.29768296281241674</v>
+      </c>
+      <c r="C8">
+        <v>0.2285484250723385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>50</v>
       </c>
-      <c r="K13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O13" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I14">
+      <c r="B9">
+        <v>0.29914938943151953</v>
+      </c>
+      <c r="C9">
+        <v>0.23317901886556028</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>60</v>
       </c>
-      <c r="K14" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L14" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M14" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N14" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O14" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="15" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I15">
+      <c r="B10">
+        <v>0.29968731803865895</v>
+      </c>
+      <c r="C10">
+        <v>0.2370269677519623</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>70</v>
       </c>
-      <c r="K15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" t="e">
-        <f ca="1">_xll.BHX_xloil(I8:I15,K6,L6,M5,N5,0.5,1)</f>
-        <v>#VALUE!</v>
+      <c r="B11">
+        <v>0.29988500320540673</v>
+      </c>
+      <c r="C11">
+        <v>0.24046720943024608</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>80</v>
+      </c>
+      <c r="B12">
+        <v>0.29995769943619105</v>
+      </c>
+      <c r="C12">
+        <v>0.24364372940945142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>90</v>
+      </c>
+      <c r="B13">
+        <v>0.29998443908663064</v>
+      </c>
+      <c r="C13">
+        <v>0.24661621405008735</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>0.29999427554032548</v>
+      </c>
+      <c r="C14">
+        <v>0.24941316087209395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>110</v>
+      </c>
+      <c r="B15">
+        <v>0.29999789409986005</v>
+      </c>
+      <c r="C15">
+        <v>0.25205121852277912</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>120</v>
+      </c>
+      <c r="B16">
+        <v>0.29999922528410666</v>
+      </c>
+      <c r="C16">
+        <v>0.25454226774569666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>130</v>
+      </c>
+      <c r="B17">
+        <v>0.29999971499814942</v>
+      </c>
+      <c r="C17">
+        <v>0.25689603935205052</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>140</v>
+      </c>
+      <c r="B18">
+        <v>0.29999989515370551</v>
+      </c>
+      <c r="C18">
+        <v>0.25912110317634063</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>150</v>
+      </c>
+      <c r="B19">
+        <v>0.29999996142920743</v>
+      </c>
+      <c r="C19">
+        <v>0.26122525995674178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>160</v>
+      </c>
+      <c r="B20">
+        <v>0.29999998581059889</v>
+      </c>
+      <c r="C20">
+        <v>0.26321571245463549</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>170</v>
+      </c>
+      <c r="B21">
+        <v>0.2999999947800111</v>
+      </c>
+      <c r="C21">
+        <v>0.26509915333004203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>180</v>
+      </c>
+      <c r="B22">
+        <v>0.29999999807967342</v>
+      </c>
+      <c r="C22">
+        <v>0.2668818202277834</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>190</v>
+      </c>
+      <c r="B23">
+        <v>0.29999999929355137</v>
+      </c>
+      <c r="C23">
+        <v>0.26856953674827427</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>200</v>
+      </c>
+      <c r="B24">
+        <v>0.29999999974011204</v>
+      </c>
+      <c r="C24">
+        <v>0.27016774635104346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>210</v>
+      </c>
+      <c r="B25">
+        <v>0.29999999990439258</v>
+      </c>
+      <c r="C25">
+        <v>0.27168154196806199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>220</v>
+      </c>
+      <c r="B26">
+        <v>0.29999999996482801</v>
+      </c>
+      <c r="C26">
+        <v>0.27311569252019052</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>230</v>
+      </c>
+      <c r="B27">
+        <v>0.29999999998706095</v>
+      </c>
+      <c r="C27">
+        <v>0.27447466693042666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>240</v>
+      </c>
+      <c r="B28">
+        <v>0.29999999999524002</v>
+      </c>
+      <c r="C28">
+        <v>0.27576265599015631</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>250</v>
+      </c>
+      <c r="B29">
+        <v>0.29999999999824895</v>
+      </c>
+      <c r="C29">
+        <v>0.27698359233181136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>260</v>
+      </c>
+      <c r="B30">
+        <v>0.29999999999935584</v>
+      </c>
+      <c r="C30">
+        <v>0.27814116870978345</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>270</v>
+      </c>
+      <c r="B31">
+        <v>0.29999999999976307</v>
+      </c>
+      <c r="C31">
+        <v>0.27923885476039506</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>280</v>
+      </c>
+      <c r="B32">
+        <v>0.29999999999991284</v>
+      </c>
+      <c r="C32">
+        <v>0.28027991238967825</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>290</v>
+      </c>
+      <c r="B33">
+        <v>0.29999999999996796</v>
+      </c>
+      <c r="C33">
+        <v>0.28126740992027205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>300</v>
+      </c>
+      <c r="B34">
+        <v>0.29999999999998822</v>
+      </c>
+      <c r="C34">
+        <v>0.28220423511412168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>310</v>
+      </c>
+      <c r="B35">
+        <v>0.29999999999999571</v>
+      </c>
+      <c r="C35">
+        <v>0.28309310717505093</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>320</v>
+      </c>
+      <c r="B36">
+        <v>0.29999999999999843</v>
+      </c>
+      <c r="C36">
+        <v>0.28393658782425996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>330</v>
+      </c>
+      <c r="B37">
+        <v>0.29999999999999938</v>
+      </c>
+      <c r="C37">
+        <v>0.28473709153210258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>340</v>
+      </c>
+      <c r="B38">
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="C38">
+        <v>0.2854968949809441</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>350</v>
+      </c>
+      <c r="B39">
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="C39">
+        <v>0.28621814582631872</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>360</v>
+      </c>
+      <c r="B40">
+        <v>0.3</v>
+      </c>
+      <c r="C40">
+        <v>0.28690287081689186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>370</v>
+      </c>
+      <c r="B41">
+        <v>0.3</v>
+      </c>
+      <c r="C41">
+        <v>0.28755298332776219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>380</v>
+      </c>
+      <c r="B42">
+        <v>0.3</v>
+      </c>
+      <c r="C42">
+        <v>0.28817029035632741</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>390</v>
+      </c>
+      <c r="B43">
+        <v>0.3</v>
+      </c>
+      <c r="C43">
+        <v>0.28875649902520778</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>400</v>
+      </c>
+      <c r="B44">
+        <v>0.3</v>
+      </c>
+      <c r="C44">
+        <v>0.28931322263249476</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>410</v>
+      </c>
+      <c r="B45">
+        <v>0.3</v>
+      </c>
+      <c r="C45">
+        <v>0.28984198628582208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>420</v>
+      </c>
+      <c r="B46">
+        <v>0.3</v>
+      </c>
+      <c r="C46">
+        <v>0.29034423215337501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>430</v>
+      </c>
+      <c r="B47">
+        <v>0.3</v>
+      </c>
+      <c r="C47">
+        <v>0.29082132436193064</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>440</v>
+      </c>
+      <c r="B48">
+        <v>0.3</v>
+      </c>
+      <c r="C48">
+        <v>0.29127455356930265</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>450</v>
+      </c>
+      <c r="B49">
+        <v>0.3</v>
+      </c>
+      <c r="C49">
+        <v>0.29170514123612584</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>460</v>
+      </c>
+      <c r="B50">
+        <v>0.3</v>
+      </c>
+      <c r="C50">
+        <v>0.29211424361971899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>